<commit_message>
Add date and time types to FieldDefinition. Add a date and time fields to ParsingPatternForDateTest.java Update ProjectSettingsTest to actually check the menu.
</commit_message>
<xml_diff>
--- a/data/DateParsing/BulkImportDateParsing.xlsx
+++ b/data/DateParsing/BulkImportDateParsing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\LabKey\git-trunk\server\testAutomation\data\DateParsing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danduffek/labkey/trunk_all/server/testAutomation/data/DateParsing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D65D53D-1603-44C5-87CC-0ED2F2911197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683365D2-9BB6-D24C-8588-7CCB87A98222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35620" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -42,9 +42,6 @@
     <t>Fifth</t>
   </si>
   <si>
-    <t>sixth</t>
-  </si>
-  <si>
     <t>23Mar2020:12:23:34</t>
   </si>
   <si>
@@ -55,12 +52,24 @@
   </si>
   <si>
     <t>23Jun2020:12:29:34</t>
+  </si>
+  <si>
+    <t>DateTimeCol</t>
+  </si>
+  <si>
+    <t>Sixth</t>
+  </si>
+  <si>
+    <t>TimeCol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -102,12 +111,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,57 +399,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="32.28515625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" ht="13.5">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="4">
+        <v>44188</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.51428240740740738</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.5">
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>43853</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.51706018518518515</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13.5">
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="C4" s="4">
+        <v>43913</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.51636574074074071</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13.5">
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="C5" s="4">
+        <v>44005</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.52053240740740747</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Clean up tests validating checking site settings vs project settings. Clean up test that uses additional pattern parsing.
</commit_message>
<xml_diff>
--- a/data/DateParsing/BulkImportDateParsing.xlsx
+++ b/data/DateParsing/BulkImportDateParsing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danduffek/labkey/trunk_all/server/testAutomation/data/DateParsing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683365D2-9BB6-D24C-8588-7CCB87A98222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FD5543-5A5D-8F44-B37C-A8B8DA6B5384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35620" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>DateCol</t>
   </si>
   <si>
-    <t>Thrid</t>
-  </si>
-  <si>
     <t>Fourth</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t>TimeCol</t>
+  </si>
+  <si>
+    <t>Third</t>
   </si>
 </sst>
 </file>
@@ -68,7 +68,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -117,7 +117,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -402,7 +402,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
@@ -419,21 +419,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4">
         <v>44188</v>
@@ -444,44 +444,44 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4">
         <v>43853</v>
       </c>
       <c r="D3" s="3">
-        <v>0.51706018518518515</v>
+        <v>1.7071759259259259E-2</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="C4" s="4">
         <v>43913</v>
       </c>
       <c r="D4" s="3">
-        <v>0.51636574074074071</v>
+        <v>0.5163888888888889</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="4">
         <v>44005</v>
       </c>
       <c r="D5" s="3">
-        <v>0.52053240740740747</v>
+        <v>0.47890046296296296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test for site-wide vs project specific import formats. Add a test that validates dates & times in a xlsx that are in string format.
</commit_message>
<xml_diff>
--- a/data/DateParsing/BulkImportDateParsing.xlsx
+++ b/data/DateParsing/BulkImportDateParsing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danduffek/labkey/trunk_all/server/testAutomation/data/DateParsing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FD5543-5A5D-8F44-B37C-A8B8DA6B5384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25E38EF-D494-5244-8A03-637B272F90C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35620" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38440" yWindow="20" windowWidth="34560" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -36,25 +36,13 @@
     <t>Fourth</t>
   </si>
   <si>
-    <t>Fifth</t>
-  </si>
-  <si>
-    <t>23Mar2020:12:23:34</t>
-  </si>
-  <si>
     <t>23Dec2020:12:20:34</t>
   </si>
   <si>
     <t>23Jan2020:12:24:34</t>
   </si>
   <si>
-    <t>23Jun2020:12:29:34</t>
-  </si>
-  <si>
     <t>DateTimeCol</t>
-  </si>
-  <si>
-    <t>Sixth</t>
   </si>
   <si>
     <t>TimeCol</t>
@@ -399,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
@@ -419,21 +407,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" s="4">
         <v>44188</v>
@@ -447,41 +435,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4">
         <v>43853</v>
       </c>
       <c r="D3" s="3">
         <v>1.7071759259259259E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4">
-        <v>43913</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.5163888888888889</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4">
-        <v>44005</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0.47890046296296296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Automation for Date-only and Time-only Fields (#1836)
</commit_message>
<xml_diff>
--- a/data/DateParsing/BulkImportDateParsing.xlsx
+++ b/data/DateParsing/BulkImportDateParsing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\LabKey\git-trunk\server\testAutomation\data\DateParsing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danduffek/labkey/trunk_all/server/testAutomation/data/DateParsing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D65D53D-1603-44C5-87CC-0ED2F2911197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A25E38EF-D494-5244-8A03-637B272F90C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38440" yWindow="20" windowWidth="34560" windowHeight="19620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -33,34 +33,31 @@
     <t>DateCol</t>
   </si>
   <si>
-    <t>Thrid</t>
-  </si>
-  <si>
     <t>Fourth</t>
   </si>
   <si>
-    <t>Fifth</t>
-  </si>
-  <si>
-    <t>sixth</t>
-  </si>
-  <si>
-    <t>23Mar2020:12:23:34</t>
-  </si>
-  <si>
     <t>23Dec2020:12:20:34</t>
   </si>
   <si>
     <t>23Jan2020:12:24:34</t>
   </si>
   <si>
-    <t>23Jun2020:12:29:34</t>
+    <t>DateTimeCol</t>
+  </si>
+  <si>
+    <t>TimeCol</t>
+  </si>
+  <si>
+    <t>Third</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -102,12 +99,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,57 +387,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="32.28515625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.1640625" style="1"/>
+    <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" style="1"/>
+    <col min="4" max="4" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" ht="13.5">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4">
+        <v>44188</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.51428240740740738</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="13.5">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="13.5">
-      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="13.5">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
+      <c r="C3" s="4">
+        <v>43853</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1.7071759259259259E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>